<commit_message>
Added Vin voltage display monitoring. Cleaned up OLED display refresh.
</commit_message>
<xml_diff>
--- a/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
+++ b/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Arduino_Projects/Encoder_Pulse_Stretcher/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD81F90-F3EE-E64F-8929-D18BC26215E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEDF26E-60D2-9E49-8506-21FBA5AF0B0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45680" yWindow="-1840" windowWidth="31160" windowHeight="18840" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
+    <workbookView xWindow="-51200" yWindow="-10340" windowWidth="48820" windowHeight="18160" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>INPUT</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>OLED CLOCK</t>
+  </si>
+  <si>
+    <t>Voltage Monitor (1/2 VIN)</t>
+  </si>
+  <si>
+    <t>The microcontroller on the Arduino NANO Every runs at 5V and it is fully electrically compatible with the original Arduino Nano designs. The headers are mapped in the same way and it is possible to substitute any Arduino Nano board with the new Arduino Nano Every.</t>
+  </si>
+  <si>
+    <t>On the software side there might be some issue with third party libraries that don't manage the pin mapping of the microcontroller; if the sketch has assembly parts inside, you should turn on the "Register Emulation" mode to emulate ATmega328P registers in the 4809 while compiling.</t>
   </si>
 </sst>
 </file>
@@ -191,7 +200,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -206,6 +215,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF4F4E4E"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -284,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -296,6 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -318,16 +334,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>55418</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28863</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>173604</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>207818</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>422</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -350,8 +366,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="228600" y="406400"/>
-          <a:ext cx="10058400" cy="7285604"/>
+          <a:off x="24632804" y="432954"/>
+          <a:ext cx="10023764" cy="7245195"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -362,16 +378,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>660401</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>25401</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>27132</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>393701</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581315</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>179103</xdr:rowOff>
+      <xdr:rowOff>193535</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -394,8 +410,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10566401" y="419100"/>
-          <a:ext cx="7988300" cy="7278403"/>
+          <a:off x="848015" y="431223"/>
+          <a:ext cx="7959436" cy="7237994"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -406,16 +422,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>101601</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>119738</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>58306</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>191896</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>120528</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9750950</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>86591</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -445,8 +461,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5880101" y="9263738"/>
-          <a:ext cx="9905999" cy="5893590"/>
+          <a:off x="12556261" y="1000078"/>
+          <a:ext cx="9692644" cy="5754013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1365,60 +1381,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F09D0F-A22B-984D-A0E9-6079E9A67F22}">
-  <dimension ref="G39:Q63"/>
+  <dimension ref="B21:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C44" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="13" max="13" width="34.5" customWidth="1"/>
+    <col min="14" max="14" width="130.1640625" customWidth="1"/>
+    <col min="15" max="15" width="28.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="39" spans="14:17" x14ac:dyDescent="0.2">
-      <c r="N39" t="s">
+    <row r="21" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" ht="23" x14ac:dyDescent="0.25">
+      <c r="N39" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" ht="23" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="14:17" x14ac:dyDescent="0.2">
-      <c r="N40" t="s">
+      <c r="N40" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>38</v>
       </c>
-      <c r="O40" t="s">
+      <c r="C41" t="s">
         <v>39</v>
       </c>
-      <c r="P40" t="s">
+      <c r="D41" t="s">
         <v>40</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="E41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="14:17" x14ac:dyDescent="0.2">
-      <c r="Q41" t="s">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="14:17" x14ac:dyDescent="0.2">
-      <c r="N42" t="s">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>45</v>
       </c>
-      <c r="O42" t="s">
+      <c r="C43" t="s">
         <v>2</v>
       </c>
-      <c r="P42" t="s">
+      <c r="D43" t="s">
         <v>44</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="E43" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G62" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G63" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doc update input encoder channels.
</commit_message>
<xml_diff>
--- a/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
+++ b/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Arduino_Projects/Encoder_Pulse_Stretcher/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEDF26E-60D2-9E49-8506-21FBA5AF0B0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D801138-77C1-8443-8A4F-0BEA8D71C54B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-10340" windowWidth="48820" windowHeight="18160" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>INPUT</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>On the software side there might be some issue with third party libraries that don't manage the pin mapping of the microcontroller; if the sketch has assembly parts inside, you should turn on the "Register Emulation" mode to emulate ATmega328P registers in the 4809 while compiling.</t>
+  </si>
+  <si>
+    <t>https://www.arduino.cc/en/Guide/NANOEvery</t>
+  </si>
+  <si>
+    <t>Encoder Input Channel A</t>
+  </si>
+  <si>
+    <t>Encoder Input Channel B</t>
   </si>
 </sst>
 </file>
@@ -1381,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F09D0F-A22B-984D-A0E9-6079E9A67F22}">
-  <dimension ref="B21:N43"/>
+  <dimension ref="B18:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="88" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,6 +1403,16 @@
     <col min="15" max="15" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="18" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="21" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M21" t="s">
         <v>47</v>
@@ -1409,6 +1428,11 @@
         <v>49</v>
       </c>
     </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N38" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="39" spans="2:14" ht="23" x14ac:dyDescent="0.25">
       <c r="N39" s="11" t="s">
         <v>50</v>
@@ -1456,7 +1480,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N38" r:id="rId1" xr:uid="{36CAD947-865F-B445-98A0-8FEE504294A3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Nano Every schematic and pinout, initial calibration at 4.72V complete.
</commit_message>
<xml_diff>
--- a/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
+++ b/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Arduino_Projects/Encoder_Pulse_Stretcher/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D801138-77C1-8443-8A4F-0BEA8D71C54B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F782FA9-6970-9740-AFA8-04F5FAC67E17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
+    <workbookView xWindow="-30000" yWindow="-1800" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>INPUT</t>
   </si>
@@ -199,6 +199,126 @@
   </si>
   <si>
     <t>Encoder Input Channel B</t>
+  </si>
+  <si>
+    <t>https://store.arduino.cc/usa/nano-every-pack</t>
+  </si>
+  <si>
+    <t>The Arduino Nano Every is based on the ATMega4809 microcontroller.</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>ATMega4809 (datasheet)</t>
+  </si>
+  <si>
+    <t>Operating Voltage</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>Input Voltage (limit)</t>
+  </si>
+  <si>
+    <t>21V</t>
+  </si>
+  <si>
+    <t>DC Current per I/O Pin</t>
+  </si>
+  <si>
+    <t>20 mA</t>
+  </si>
+  <si>
+    <t>DC Current for 3.3V Pin</t>
+  </si>
+  <si>
+    <t>50 mA</t>
+  </si>
+  <si>
+    <t>Clock Speed</t>
+  </si>
+  <si>
+    <t>20MHz</t>
+  </si>
+  <si>
+    <t>CPU Flash Memory</t>
+  </si>
+  <si>
+    <t>48KB (ATMega4809)</t>
+  </si>
+  <si>
+    <t>SRAM</t>
+  </si>
+  <si>
+    <t>6KB (ATMega4809)</t>
+  </si>
+  <si>
+    <t>EEPROM</t>
+  </si>
+  <si>
+    <t>256byte (ATMega4809)</t>
+  </si>
+  <si>
+    <t>PWM Pins</t>
+  </si>
+  <si>
+    <t>5 (D3, D5, D6, D9, D10)</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>Analog Input Pins</t>
+  </si>
+  <si>
+    <t>8 (ADC 10 bit)</t>
+  </si>
+  <si>
+    <t>Analog Output Pins</t>
+  </si>
+  <si>
+    <t>Only through PWM (no DAC)</t>
+  </si>
+  <si>
+    <t>External Interrupts</t>
+  </si>
+  <si>
+    <t>all digital pins</t>
+  </si>
+  <si>
+    <t>LED_BUILTIN</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>Uses the ATSAMD11D14A (datasheet)</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>45 mm</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>18 mm</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>5 gr (with headers)</t>
   </si>
 </sst>
 </file>
@@ -209,7 +329,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -229,6 +349,12 @@
       <sz val="18"/>
       <color rgb="FF4F4E4E"/>
       <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF434F54"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -308,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -321,6 +447,15 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1390,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F09D0F-A22B-984D-A0E9-6079E9A67F22}">
-  <dimension ref="B18:N43"/>
+  <dimension ref="B18:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="88" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1459,13 +1594,20 @@
       <c r="E41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N41" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" ht="22" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M42" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N42" s="13"/>
+    </row>
+    <row r="43" spans="2:14" ht="22" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>45</v>
       </c>
@@ -1477,13 +1619,186 @@
       </c>
       <c r="E43" t="s">
         <v>43</v>
+      </c>
+      <c r="M43" s="12"/>
+      <c r="N43" s="13"/>
+    </row>
+    <row r="44" spans="2:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M44" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="N44" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M45" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M46" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M47" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="N47" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M48" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M49" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M50" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="N50" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M51" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M52" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M53" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N53" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M54" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="N54" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M55" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="N55" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M56" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="N56" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M57" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M58" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N58" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M59" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="N59" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M60" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="N60" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M61" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="N61" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M62" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="N62" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M63" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="N63" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M64" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="N64" s="12" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N38" r:id="rId1" xr:uid="{36CAD947-865F-B445-98A0-8FEE504294A3}"/>
+    <hyperlink ref="N41" r:id="rId2" xr:uid="{6B73E62E-ED85-E448-A532-85D576C362D6}"/>
+    <hyperlink ref="N44" r:id="rId3" display="https://content.arduino.cc/assets/Nano-Every_processor-48-pin-Data-Sheet-megaAVR-0-series-DS40002016B.pdf" xr:uid="{6A1D8C37-3229-9147-9B62-7F0F0A18D8A0}"/>
+    <hyperlink ref="N61" r:id="rId4" display="https://content.arduino.cc/assets/Nano-Every_USB-Serial_Atmel-42363-SAM-D11_Datasheet.pdf" xr:uid="{28AD1BC9-59DF-5E49-8FA4-36373CF9B5C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update pin choices for outgoing encoder pulses.
</commit_message>
<xml_diff>
--- a/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
+++ b/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Arduino_Projects/Encoder_Pulse_Stretcher/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F782FA9-6970-9740-AFA8-04F5FAC67E17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF0AF9F-693D-8941-BFA0-378A117F4467}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30000" yWindow="-1800" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
+    <workbookView xWindow="-50580" yWindow="-6500" windowWidth="38260" windowHeight="24100" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
   <si>
     <t>INPUT</t>
   </si>
@@ -319,6 +319,33 @@
   </si>
   <si>
     <t>5 gr (with headers)</t>
+  </si>
+  <si>
+    <t>Left edge of LVCB</t>
+  </si>
+  <si>
+    <t>SHIELD</t>
+  </si>
+  <si>
+    <t>CHN A</t>
+  </si>
+  <si>
+    <t>CHN B</t>
+  </si>
+  <si>
+    <t>GND to breadboard</t>
+  </si>
+  <si>
+    <t>Vin to 5V breadboard</t>
+  </si>
+  <si>
+    <t>Encoder OUTPUT Channel B</t>
+  </si>
+  <si>
+    <t>Encoder OUTPUT Channel A</t>
+  </si>
+  <si>
+    <t>Button</t>
   </si>
 </sst>
 </file>
@@ -566,61 +593,176 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>58306</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>191896</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>50798</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>9750950</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>86591</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>173880</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>186267</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B08A649-CE2A-D045-BFF8-835849F832CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E67DDEA5-2225-0048-8DA4-97CCB66EAD2B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="12556261" y="1000078"/>
-          <a:ext cx="9692644" cy="5754013"/>
+          <a:off x="37168665" y="1100667"/>
+          <a:ext cx="9250149" cy="6197600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>186267</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>118532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>356711</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>49903</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75917609-662C-354B-87AF-C4DDCB921B8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="40623067" y="931332"/>
+          <a:ext cx="5978578" cy="6433771"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>13309601</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33867</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2DC758C-3DAC-AD42-88AB-2BE94C8D3B31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12606867" y="1303867"/>
+          <a:ext cx="13284201" cy="4826000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>118531</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>13301460</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>135467</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3FC8B52-7174-1A40-9AA2-19BA083942F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12699998" y="6146800"/>
+          <a:ext cx="13182929" cy="1710267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1525,278 +1667,342 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F09D0F-A22B-984D-A0E9-6079E9A67F22}">
-  <dimension ref="B18:N64"/>
+  <dimension ref="G3:AE67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView tabSelected="1" topLeftCell="N8" zoomScale="134" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="13" max="13" width="34.5" customWidth="1"/>
-    <col min="14" max="14" width="130.1640625" customWidth="1"/>
+    <col min="14" max="14" width="175.83203125" customWidth="1"/>
     <col min="15" max="15" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="18" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M18" t="s">
+    <row r="3" spans="15:31" x14ac:dyDescent="0.2">
+      <c r="AE3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="15:31" x14ac:dyDescent="0.2">
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="15:31" x14ac:dyDescent="0.2">
+      <c r="AC13">
+        <v>2</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="15:31" x14ac:dyDescent="0.2">
+      <c r="O14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="15:31" x14ac:dyDescent="0.2">
+      <c r="O15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="15:31" x14ac:dyDescent="0.2">
+      <c r="O16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M19" t="s">
+    <row r="17" spans="13:30" x14ac:dyDescent="0.2">
+      <c r="O17" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="AC17">
+        <v>3</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="13:30" x14ac:dyDescent="0.2">
       <c r="M21" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="AC21">
+        <v>4</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="13:30" x14ac:dyDescent="0.2">
       <c r="M22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="13:30" x14ac:dyDescent="0.2">
       <c r="M24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="N38" s="10" t="s">
+      <c r="O24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="13:30" x14ac:dyDescent="0.2">
+      <c r="O25" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC25">
+        <v>5</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="13:30" x14ac:dyDescent="0.2">
+      <c r="M28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>38</v>
+      </c>
+      <c r="H41" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41" t="s">
+        <v>40</v>
+      </c>
+      <c r="J41" t="s">
+        <v>41</v>
+      </c>
+      <c r="N41" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="2:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="N39" s="11" t="s">
+    <row r="42" spans="7:14" ht="23" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>42</v>
+      </c>
+      <c r="N42" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="2:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>46</v>
-      </c>
-      <c r="N40" s="11" t="s">
+    <row r="43" spans="7:14" ht="23" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>45</v>
+      </c>
+      <c r="H43" t="s">
+        <v>2</v>
+      </c>
+      <c r="I43" t="s">
+        <v>44</v>
+      </c>
+      <c r="J43" t="s">
+        <v>43</v>
+      </c>
+      <c r="N43" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" t="s">
-        <v>41</v>
-      </c>
-      <c r="N41" s="10" t="s">
+    <row r="44" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="N44" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="2:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
-        <v>42</v>
-      </c>
-      <c r="M42" s="12" t="s">
+    <row r="45" spans="7:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M45" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="N42" s="13"/>
-    </row>
-    <row r="43" spans="2:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>44</v>
-      </c>
-      <c r="E43" t="s">
-        <v>43</v>
-      </c>
-      <c r="M43" s="12"/>
-      <c r="N43" s="13"/>
-    </row>
-    <row r="44" spans="2:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="M44" s="12" t="s">
+      <c r="N45" s="13"/>
+    </row>
+    <row r="46" spans="7:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M46" s="12"/>
+      <c r="N46" s="13"/>
+    </row>
+    <row r="47" spans="7:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M47" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="N44" s="14" t="s">
+      <c r="N47" s="14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="2:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="M45" s="12" t="s">
+    <row r="48" spans="7:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M48" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="N45" s="12" t="s">
+      <c r="N48" s="12" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="M46" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N46" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="M47" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N47" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="M48" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="N48" s="12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="49" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M49" s="12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="N49" s="12" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M50" s="12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M51" s="12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M52" s="12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="N52" s="12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M53" s="12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M54" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="N54" s="12">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="N54" s="12" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M55" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="N55" s="12">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="N55" s="12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M56" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="N56" s="12">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="N56" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M57" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="N57" s="12" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="N57" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M58" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="N58" s="12" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="N58" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M59" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="N59" s="12" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="N59" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M60" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="N60" s="12">
-        <v>13</v>
+        <v>80</v>
+      </c>
+      <c r="N60" s="12" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M61" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="N61" s="14" t="s">
-        <v>88</v>
+        <v>82</v>
+      </c>
+      <c r="N61" s="12" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M62" s="12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M63" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="N63" s="12" t="s">
-        <v>92</v>
+        <v>86</v>
+      </c>
+      <c r="N63" s="12">
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M64" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="N64" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M65" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="N65" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M66" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="N66" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="M67" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="N64" s="12" t="s">
+      <c r="N67" s="12" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N38" r:id="rId1" xr:uid="{36CAD947-865F-B445-98A0-8FEE504294A3}"/>
-    <hyperlink ref="N41" r:id="rId2" xr:uid="{6B73E62E-ED85-E448-A532-85D576C362D6}"/>
-    <hyperlink ref="N44" r:id="rId3" display="https://content.arduino.cc/assets/Nano-Every_processor-48-pin-Data-Sheet-megaAVR-0-series-DS40002016B.pdf" xr:uid="{6A1D8C37-3229-9147-9B62-7F0F0A18D8A0}"/>
-    <hyperlink ref="N61" r:id="rId4" display="https://content.arduino.cc/assets/Nano-Every_USB-Serial_Atmel-42363-SAM-D11_Datasheet.pdf" xr:uid="{28AD1BC9-59DF-5E49-8FA4-36373CF9B5C0}"/>
+    <hyperlink ref="N41" r:id="rId1" xr:uid="{36CAD947-865F-B445-98A0-8FEE504294A3}"/>
+    <hyperlink ref="N44" r:id="rId2" xr:uid="{6B73E62E-ED85-E448-A532-85D576C362D6}"/>
+    <hyperlink ref="N47" r:id="rId3" display="https://content.arduino.cc/assets/Nano-Every_processor-48-pin-Data-Sheet-megaAVR-0-series-DS40002016B.pdf" xr:uid="{6A1D8C37-3229-9147-9B62-7F0F0A18D8A0}"/>
+    <hyperlink ref="N64" r:id="rId4" display="https://content.arduino.cc/assets/Nano-Every_USB-Serial_Atmel-42363-SAM-D11_Datasheet.pdf" xr:uid="{28AD1BC9-59DF-5E49-8FA4-36373CF9B5C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId5"/>

</xml_diff>

<commit_message>
Encoder library change. Do not use Arduino Encoder. Use simpler encoder functions in my source, not as library. Add tach speed reading.
</commit_message>
<xml_diff>
--- a/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
+++ b/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Arduino_Projects/Encoder_Pulse_Stretcher/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF0AF9F-693D-8941-BFA0-378A117F4467}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D752649-DE77-6C4F-82A9-AB8D08713E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50580" yWindow="-6500" windowWidth="38260" windowHeight="24100" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
   <si>
     <t>INPUT</t>
   </si>
@@ -346,6 +346,24 @@
   </si>
   <si>
     <t>Button</t>
+  </si>
+  <si>
+    <t>ALTERNATE FOR TESTING</t>
+  </si>
+  <si>
+    <t>WHT</t>
+  </si>
+  <si>
+    <t>GRN</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>PUR</t>
   </si>
 </sst>
 </file>
@@ -461,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -483,6 +501,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -759,6 +778,50 @@
         <a:xfrm>
           <a:off x="12699998" y="6146800"/>
           <a:ext cx="13182929" cy="1710267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>16934</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>546365</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>33866</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6344E441-8514-D943-BF41-04986EA4575D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="846667" y="11988800"/>
+          <a:ext cx="5507831" cy="8246533"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1667,10 +1730,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F09D0F-A22B-984D-A0E9-6079E9A67F22}">
-  <dimension ref="G3:AE67"/>
+  <dimension ref="B3:AE67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N8" zoomScale="134" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1767,12 +1830,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G40" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G41" t="s">
         <v>38</v>
       </c>
@@ -1789,7 +1852,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="7:14" ht="23" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" ht="23" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
         <v>42</v>
       </c>
@@ -1797,7 +1860,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="7:14" ht="23" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" ht="23" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
         <v>45</v>
       </c>
@@ -1814,22 +1877,25 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
       <c r="N44" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="7:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M45" s="12" t="s">
         <v>56</v>
       </c>
       <c r="N45" s="13"/>
     </row>
-    <row r="46" spans="7:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M46" s="12"/>
       <c r="N46" s="13"/>
     </row>
-    <row r="47" spans="7:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>104</v>
+      </c>
       <c r="M47" s="12" t="s">
         <v>57</v>
       </c>
@@ -1837,7 +1903,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="7:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48" t="s">
+        <v>40</v>
+      </c>
       <c r="M48" s="12" t="s">
         <v>59</v>
       </c>
@@ -1845,7 +1926,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" t="s">
+        <v>108</v>
+      </c>
       <c r="M49" s="12" t="s">
         <v>61</v>
       </c>
@@ -1853,7 +1946,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M50" s="12" t="s">
         <v>63</v>
       </c>
@@ -1861,7 +1954,19 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51" t="s">
+        <v>106</v>
+      </c>
       <c r="M51" s="12" t="s">
         <v>65</v>
       </c>
@@ -1869,7 +1974,19 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>60</v>
+      </c>
+      <c r="E52" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" t="s">
+        <v>108</v>
+      </c>
       <c r="M52" s="12" t="s">
         <v>67</v>
       </c>
@@ -1877,7 +1994,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M53" s="12" t="s">
         <v>69</v>
       </c>
@@ -1885,7 +2002,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M54" s="12" t="s">
         <v>71</v>
       </c>
@@ -1893,7 +2010,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M55" s="12" t="s">
         <v>73</v>
       </c>
@@ -1901,7 +2018,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M56" s="12" t="s">
         <v>75</v>
       </c>
@@ -1909,7 +2026,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M57" s="12" t="s">
         <v>77</v>
       </c>
@@ -1917,7 +2034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M58" s="12" t="s">
         <v>78</v>
       </c>
@@ -1925,7 +2042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M59" s="12" t="s">
         <v>79</v>
       </c>
@@ -1933,7 +2050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M60" s="12" t="s">
         <v>80</v>
       </c>
@@ -1941,7 +2058,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M61" s="12" t="s">
         <v>82</v>
       </c>
@@ -1949,7 +2066,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M62" s="12" t="s">
         <v>84</v>
       </c>
@@ -1957,7 +2074,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M63" s="12" t="s">
         <v>86</v>
       </c>
@@ -1965,7 +2082,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="13:14" ht="22" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M64" s="12" t="s">
         <v>87</v>
       </c>
@@ -2005,6 +2122,7 @@
     <hyperlink ref="N64" r:id="rId4" display="https://content.arduino.cc/assets/Nano-Every_USB-Serial_Atmel-42363-SAM-D11_Datasheet.pdf" xr:uid="{28AD1BC9-59DF-5E49-8FA4-36373CF9B5C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pulse stretcher working in the B6. Added DigitalWriteFast in src folder.
</commit_message>
<xml_diff>
--- a/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
+++ b/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Arduino_Projects/Encoder_Pulse_Stretcher/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D752649-DE77-6C4F-82A9-AB8D08713E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BC1669-67CE-6E48-9D7C-303983BAC351}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
+    <workbookView xWindow="0" yWindow="5280" windowWidth="29000" windowHeight="22680" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="118">
   <si>
     <t>INPUT</t>
   </si>
@@ -364,6 +364,30 @@
   </si>
   <si>
     <t>PUR</t>
+  </si>
+  <si>
+    <t>Measure the time between pulses.</t>
+  </si>
+  <si>
+    <t>As long as the incoming encoder is moving</t>
+  </si>
+  <si>
+    <t>Multiply the incoming pulses time delta by 7/3.</t>
+  </si>
+  <si>
+    <t>Increment the output of the virtual encoder at that new rate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The blender encoders need the internal pull-up on the </t>
+  </si>
+  <si>
+    <t>Arduino to be enabled to drive a signal.</t>
+  </si>
+  <si>
+    <t>Input encoder triggers pin state-change interrupt for precision.</t>
+  </si>
+  <si>
+    <t>Output encoder is driven by time-based interrupt with 1ms period to allow output state change in between the input encoder pulses.</t>
   </si>
 </sst>
 </file>
@@ -403,7 +427,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,6 +437,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -502,6 +532,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1130,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7F9C67-679F-0B4D-AEEB-27155B435AE5}">
-  <dimension ref="C1:AW46"/>
+  <dimension ref="A1:AW53"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,7 +1172,7 @@
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:49" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="J1" s="7" t="s">
         <v>14</v>
       </c>
@@ -1173,556 +1204,658 @@
       <c r="AJ1" s="7"/>
       <c r="AK1" s="7"/>
     </row>
-    <row r="2" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="D2" t="s">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="16"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="16"/>
+      <c r="AK2" s="16"/>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="3"/>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="5"/>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="3"/>
-      <c r="AL3" s="4"/>
-      <c r="AM3" s="5"/>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="3"/>
-      <c r="AP3" s="4"/>
-      <c r="AQ3" s="5"/>
-      <c r="AR3" s="6"/>
-      <c r="AS3" s="3"/>
-      <c r="AT3" s="4"/>
-      <c r="AU3" s="5"/>
-      <c r="AV3" s="6"/>
-      <c r="AW3" s="3"/>
-    </row>
-    <row r="5" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="H5" t="s">
+      <c r="J4" s="4"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="6"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="5"/>
+      <c r="AV4" s="6"/>
+      <c r="AW4" s="3"/>
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="5"/>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="3"/>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="5"/>
-      <c r="AO5" s="6"/>
-      <c r="AP5" s="3"/>
-      <c r="AQ5" s="4"/>
-      <c r="AR5" s="5"/>
-      <c r="AS5" s="6"/>
-      <c r="AT5" s="3"/>
-      <c r="AU5" s="4"/>
-      <c r="AV5" s="5"/>
-      <c r="AW5" s="6"/>
-    </row>
-    <row r="7" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="D7" t="s">
+      <c r="J6" s="3"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="6"/>
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="5"/>
+      <c r="AW6" s="6"/>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
         <v>17</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>0</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>1</v>
       </c>
-      <c r="Q15">
+      <c r="Q16">
         <v>2</v>
       </c>
-      <c r="U15">
+      <c r="U16">
         <v>3</v>
       </c>
-      <c r="Y15">
+      <c r="Y16">
         <v>4</v>
       </c>
-      <c r="AC15">
+      <c r="AC16">
         <v>5</v>
       </c>
-      <c r="AG15">
+      <c r="AG16">
         <v>6</v>
       </c>
-      <c r="AK15">
+      <c r="AK16">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="8"/>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8"/>
-      <c r="AE16" s="8"/>
-      <c r="AF16" s="8"/>
-      <c r="AG16" s="8"/>
-      <c r="AH16" s="8"/>
-      <c r="AI16" s="8"/>
-      <c r="AJ16" s="8"/>
-      <c r="AK16" s="8"/>
-      <c r="AL16" s="8"/>
-      <c r="AM16" s="8"/>
-      <c r="AN16" s="8"/>
-      <c r="AO16" s="8"/>
-      <c r="AP16" s="8"/>
-      <c r="AQ16" s="8"/>
-      <c r="AR16" s="8"/>
-      <c r="AS16" s="8"/>
-      <c r="AT16" s="8"/>
-      <c r="AU16" s="8"/>
-      <c r="AV16" s="8"/>
-      <c r="AW16" s="8"/>
-    </row>
-    <row r="17" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8"/>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="8"/>
+      <c r="AE17" s="8"/>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="8"/>
+      <c r="AI17" s="8"/>
+      <c r="AJ17" s="8"/>
+      <c r="AK17" s="8"/>
+      <c r="AL17" s="8"/>
+      <c r="AM17" s="8"/>
+      <c r="AN17" s="8"/>
+      <c r="AO17" s="8"/>
+      <c r="AP17" s="8"/>
+      <c r="AQ17" s="8"/>
+      <c r="AR17" s="8"/>
+      <c r="AS17" s="8"/>
+      <c r="AT17" s="8"/>
+      <c r="AU17" s="8"/>
+      <c r="AV17" s="8"/>
+      <c r="AW17" s="8"/>
+    </row>
+    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
         <v>11</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>0</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>1</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>2</v>
       </c>
-      <c r="L17">
+      <c r="L18">
         <v>3</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>4</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>5</v>
       </c>
-      <c r="O17">
+      <c r="O18">
         <v>6</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>7</v>
       </c>
-      <c r="Q17">
+      <c r="Q18">
         <v>8</v>
       </c>
-      <c r="R17">
+      <c r="R18">
         <v>9</v>
       </c>
-      <c r="S17">
+      <c r="S18">
         <v>10</v>
       </c>
-      <c r="T17">
+      <c r="T18">
         <v>11</v>
       </c>
-      <c r="U17">
+      <c r="U18">
         <v>12</v>
       </c>
-      <c r="V17">
+      <c r="V18">
         <v>13</v>
       </c>
-      <c r="W17">
+      <c r="W18">
         <v>14</v>
       </c>
-      <c r="X17">
+      <c r="X18">
         <v>15</v>
       </c>
-      <c r="Y17">
+      <c r="Y18">
         <v>16</v>
       </c>
-      <c r="Z17">
+      <c r="Z18">
         <v>17</v>
       </c>
-      <c r="AA17">
+      <c r="AA18">
         <v>18</v>
       </c>
-      <c r="AB17">
+      <c r="AB18">
         <v>19</v>
       </c>
-      <c r="AC17">
+      <c r="AC18">
         <v>20</v>
       </c>
-      <c r="AD17">
+      <c r="AD18">
         <v>21</v>
       </c>
-      <c r="AE17">
+      <c r="AE18">
         <v>22</v>
       </c>
-      <c r="AF17">
+      <c r="AF18">
         <v>23</v>
       </c>
-      <c r="AG17">
+      <c r="AG18">
         <v>24</v>
       </c>
-      <c r="AH17">
+      <c r="AH18">
         <v>25</v>
       </c>
-      <c r="AI17">
+      <c r="AI18">
         <v>26</v>
       </c>
-      <c r="AJ17">
+      <c r="AJ18">
         <v>27</v>
       </c>
-      <c r="AK17">
+      <c r="AK18">
         <v>28</v>
       </c>
-      <c r="AL17">
+      <c r="AL18">
         <v>29</v>
       </c>
-      <c r="AM17">
+      <c r="AM18">
         <v>30</v>
       </c>
-      <c r="AN17">
+      <c r="AN18">
         <v>31</v>
       </c>
-      <c r="AO17">
+      <c r="AO18">
         <v>32</v>
       </c>
-      <c r="AP17">
+      <c r="AP18">
         <v>33</v>
       </c>
-      <c r="AQ17">
+      <c r="AQ18">
         <v>34</v>
       </c>
-      <c r="AR17">
+      <c r="AR18">
         <v>35</v>
       </c>
-      <c r="AS17">
+      <c r="AS18">
         <v>36</v>
       </c>
-      <c r="AT17">
+      <c r="AT18">
         <v>37</v>
       </c>
-      <c r="AU17">
+      <c r="AU18">
         <v>38</v>
       </c>
-      <c r="AV17">
+      <c r="AV18">
         <v>39</v>
       </c>
-      <c r="AW17">
+      <c r="AW18">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="7"/>
-      <c r="AC19" s="7"/>
-      <c r="AD19" s="7"/>
-      <c r="AE19" s="7"/>
-      <c r="AF19" s="7"/>
-      <c r="AG19" s="7"/>
-      <c r="AH19" s="7"/>
-      <c r="AI19" s="7"/>
-      <c r="AJ19" s="7"/>
-      <c r="AK19" s="7"/>
-    </row>
-    <row r="20" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="D20" t="s">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="7"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="7"/>
+      <c r="AJ20" s="7"/>
+      <c r="AK20" s="7"/>
+    </row>
+    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="16"/>
+      <c r="X21" s="16"/>
+      <c r="Y21" s="16"/>
+      <c r="Z21" s="16"/>
+      <c r="AA21" s="16"/>
+      <c r="AB21" s="16"/>
+      <c r="AC21" s="16"/>
+      <c r="AD21" s="16"/>
+      <c r="AE21" s="16"/>
+      <c r="AF21" s="16"/>
+      <c r="AG21" s="16"/>
+      <c r="AH21" s="16"/>
+      <c r="AI21" s="16"/>
+      <c r="AJ21" s="16"/>
+      <c r="AK21" s="16"/>
+    </row>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="D21" t="s">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H23" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="4"/>
-      <c r="AE21" s="5"/>
-      <c r="AF21" s="5"/>
-      <c r="AG21" s="5"/>
-      <c r="AH21" s="5"/>
-      <c r="AI21" s="6"/>
-      <c r="AJ21" s="3"/>
-      <c r="AK21" s="3"/>
-      <c r="AL21" s="3"/>
-      <c r="AM21" s="3"/>
-    </row>
-    <row r="23" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="H23" t="s">
+      <c r="J23" s="4"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
+      <c r="AG23" s="5"/>
+      <c r="AH23" s="5"/>
+      <c r="AI23" s="6"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3"/>
+    </row>
+    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="C29">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="C31">
         <v>5000</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="C30" s="2">
-        <f>C29/60</f>
+    <row r="32" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="C32" s="2">
+        <f>C31/60</f>
         <v>83.333333333333329</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="C31">
+    <row r="33" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C33">
         <v>7</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="3:49" x14ac:dyDescent="0.2">
-      <c r="C32" s="2">
-        <f>C30*C31</f>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C34" s="2">
+        <f>C32*C33</f>
         <v>583.33333333333326</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D34" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C33" s="1">
-        <f>1/C32</f>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C35" s="1">
+        <f>1/C34</f>
         <v>1.7142857142857144E-3</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D35" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="D35" t="s">
+    <row r="37" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C36" s="9">
-        <f>C33/21</f>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C38" s="9">
+        <f>C35/21</f>
         <v>8.163265306122449E-5</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="D39" t="s">
+    <row r="41" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
         <v>33</v>
       </c>
-      <c r="L39" s="10" t="s">
+      <c r="L41" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C40">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C42">
         <f>1/13</f>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C41">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C43">
         <f>79/(2^10)</f>
         <v>7.71484375E-2</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C43">
+    <row r="45" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C45">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D45" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C44">
-        <v>341</v>
-      </c>
-      <c r="D44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C45">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="46" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C46">
-        <f>C44/(2^C45)</f>
+        <v>341</v>
+      </c>
+      <c r="D46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <f>C46/(2^C47)</f>
         <v>0.3330078125</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L39" r:id="rId1" xr:uid="{D8A7C31B-2437-764D-A2D1-FA358FF33EC8}"/>
+    <hyperlink ref="L41" r:id="rId1" xr:uid="{D8A7C31B-2437-764D-A2D1-FA358FF33EC8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1732,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F09D0F-A22B-984D-A0E9-6079E9A67F22}">
   <dimension ref="B3:AE67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1831,11 +1964,17 @@
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>114</v>
+      </c>
       <c r="G40" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>115</v>
+      </c>
       <c r="G41" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Clarify in/out encoder interrupt usage
</commit_message>
<xml_diff>
--- a/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
+++ b/Documentation/Encoder Pulse Stretcher Design Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Arduino_Projects/Encoder_Pulse_Stretcher/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BC1669-67CE-6E48-9D7C-303983BAC351}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10849A7-5CD4-CA43-B901-D5B69F4C427B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5280" windowWidth="29000" windowHeight="22680" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
+    <workbookView xWindow="0" yWindow="5260" windowWidth="29000" windowHeight="22680" xr2:uid="{FA96FA07-84D8-FE4C-877A-3F1E75D5DA34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="119">
   <si>
     <t>INPUT</t>
   </si>
@@ -66,9 +66,6 @@
     <t>RPS</t>
   </si>
   <si>
-    <t>Period</t>
-  </si>
-  <si>
     <t>TICK (1 ms)</t>
   </si>
   <si>
@@ -388,6 +385,12 @@
   </si>
   <si>
     <t>Output encoder is driven by time-based interrupt with 1ms period to allow output state change in between the input encoder pulses.</t>
+  </si>
+  <si>
+    <t>Period for one channel</t>
+  </si>
+  <si>
+    <t>Quadrature narrows the period by 4x. So the output encoder resolution should be close to 400us.</t>
   </si>
 </sst>
 </file>
@@ -1161,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7F9C67-679F-0B4D-AEEB-27155B435AE5}">
-  <dimension ref="A1:AW53"/>
+  <dimension ref="A1:AW54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1174,7 +1177,7 @@
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="J1" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
@@ -1206,7 +1209,7 @@
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1345,51 +1348,51 @@
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1461,7 +1464,7 @@
     </row>
     <row r="18" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1619,7 +1622,7 @@
     </row>
     <row r="21" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -1708,12 +1711,12 @@
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:49" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:49" x14ac:dyDescent="0.2">
@@ -1738,7 +1741,7 @@
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.2">
@@ -1747,7 +1750,7 @@
         <v>583.33333333333326</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.2">
@@ -1756,106 +1759,115 @@
         <v>1.7142857142857144E-3</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="D37" t="s">
-        <v>26</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C36" s="1">
+        <f>C35/4</f>
+        <v>4.285714285714286E-4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C38" s="9">
+      <c r="D38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C39" s="9">
         <f>C35/21</f>
         <v>8.163265306122449E-5</v>
       </c>
-      <c r="D38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="D41" t="s">
-        <v>33</v>
-      </c>
-      <c r="L41" s="10" t="s">
-        <v>30</v>
+      <c r="D39" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C42">
+      <c r="D42" t="s">
+        <v>32</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C43">
         <f>1/13</f>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="D42" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C43">
+      <c r="D43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C44">
         <f>79/(2^10)</f>
         <v>7.71484375E-2</v>
       </c>
-      <c r="D43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C45">
+      <c r="D44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C46">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D45" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C46">
-        <v>341</v>
-      </c>
       <c r="D46" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C47">
-        <v>10</v>
+        <v>341</v>
       </c>
       <c r="D47" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C48">
-        <f>C46/(2^C47)</f>
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <f>C47/(2^C48)</f>
         <v>0.3330078125</v>
       </c>
-      <c r="D48" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D50" t="s">
+      <c r="D49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D51" t="s">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D52" t="s">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D53" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L41" r:id="rId1" xr:uid="{D8A7C31B-2437-764D-A2D1-FA358FF33EC8}"/>
+    <hyperlink ref="L42" r:id="rId1" xr:uid="{D8A7C31B-2437-764D-A2D1-FA358FF33EC8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1878,7 +1890,7 @@
   <sheetData>
     <row r="3" spans="15:31" x14ac:dyDescent="0.2">
       <c r="AE3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="15:31" x14ac:dyDescent="0.2">
@@ -1886,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="AD10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="15:31" x14ac:dyDescent="0.2">
@@ -1894,136 +1906,136 @@
         <v>2</v>
       </c>
       <c r="AD13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="15:31" x14ac:dyDescent="0.2">
       <c r="O14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="15:31" x14ac:dyDescent="0.2">
       <c r="O15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="15:31" x14ac:dyDescent="0.2">
       <c r="O16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="13:30" x14ac:dyDescent="0.2">
       <c r="O17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AC17">
         <v>3</v>
       </c>
       <c r="AD17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="13:30" x14ac:dyDescent="0.2">
       <c r="M21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AC21">
         <v>4</v>
       </c>
       <c r="AD21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="13:30" x14ac:dyDescent="0.2">
       <c r="M22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="13:30" x14ac:dyDescent="0.2">
       <c r="M24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="13:30" x14ac:dyDescent="0.2">
       <c r="O25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC25">
         <v>5</v>
       </c>
       <c r="AD25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="13:30" x14ac:dyDescent="0.2">
       <c r="M28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" t="s">
         <v>38</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>39</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>40</v>
       </c>
-      <c r="J41" t="s">
-        <v>41</v>
-      </c>
       <c r="N41" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="2:14" ht="23" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N42" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="2:14" ht="23" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H43" t="s">
         <v>2</v>
       </c>
       <c r="I43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N43" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.2">
       <c r="N44" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="2:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M45" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N45" s="13"/>
     </row>
@@ -2033,36 +2045,36 @@
     </row>
     <row r="47" spans="2:14" ht="22" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M47" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N47" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="N47" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="48" spans="2:14" ht="22" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" t="s">
         <v>105</v>
       </c>
-      <c r="D48" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="F48" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="F48" s="15" t="s">
-        <v>107</v>
-      </c>
       <c r="G48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M48" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="N48" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="N48" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="49" spans="3:14" ht="22" x14ac:dyDescent="0.25">
@@ -2070,47 +2082,47 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
       </c>
       <c r="G49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M49" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="N49" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="N49" s="12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="50" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M50" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="N50" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="N50" s="12" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="51" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" t="s">
+        <v>108</v>
+      </c>
+      <c r="G51" t="s">
         <v>105</v>
       </c>
-      <c r="D51" t="s">
-        <v>41</v>
-      </c>
-      <c r="E51" t="s">
-        <v>109</v>
-      </c>
-      <c r="G51" t="s">
-        <v>106</v>
-      </c>
       <c r="M51" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="N51" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="N51" s="12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="52" spans="3:14" ht="22" x14ac:dyDescent="0.25">
@@ -2118,56 +2130,56 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
       </c>
       <c r="G52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="N52" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="N52" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="53" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M53" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N53" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="N53" s="12" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="54" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M54" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="N54" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="N54" s="12" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="55" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M55" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="N55" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="N55" s="12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="56" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M56" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="N56" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="N56" s="12" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="57" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M57" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N57" s="12">
         <v>1</v>
@@ -2175,7 +2187,7 @@
     </row>
     <row r="58" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M58" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N58" s="12">
         <v>1</v>
@@ -2183,7 +2195,7 @@
     </row>
     <row r="59" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M59" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N59" s="12">
         <v>1</v>
@@ -2191,31 +2203,31 @@
     </row>
     <row r="60" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M60" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="N60" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="N60" s="12" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="61" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M61" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N61" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="N61" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="62" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M62" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="N62" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="N62" s="12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="63" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M63" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N63" s="12">
         <v>13</v>
@@ -2223,34 +2235,34 @@
     </row>
     <row r="64" spans="3:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M64" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="N64" s="14" t="s">
         <v>87</v>
-      </c>
-      <c r="N64" s="14" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="65" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M65" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="N65" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="N65" s="12" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="66" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M66" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="N66" s="12" t="s">
         <v>91</v>
-      </c>
-      <c r="N66" s="12" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="67" spans="13:14" ht="22" x14ac:dyDescent="0.25">
       <c r="M67" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="N67" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="N67" s="12" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>